<commit_message>
direct sell option added
</commit_message>
<xml_diff>
--- a/اصلاح.xlsx
+++ b/اصلاح.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3126C11-75C1-49DE-87B7-6FD27585A864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD4EC25-33DD-4C94-9F03-778A519240BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">ایجاد پشتیبان از بانک اطلاعاتی بصورت فشرده و با درج نام فایل با تاریخ و ساعت </t>
   </si>
@@ -34,43 +35,19 @@
     <t>در صفحه افزودن کالاهای بسته بندی شده در فهرستش تعداد کالاهای بسته بندی شده موجود در ستونی نمایش داده شود  و یا در گزارشی فهرست موجودی کلیه کالاهای بسته بندی شده نمایش داده شود</t>
   </si>
   <si>
-    <t>enter index</t>
-  </si>
-  <si>
-    <t>history problem</t>
-  </si>
-  <si>
-    <t>virayesh tooye parte modiriate kala</t>
-  </si>
-  <si>
     <t>صفحه اصلی برنامه را بسته می شود ولی فرم مهای زیر مجموعه که قبلا باز بوده ، کماکلن باز می ماند</t>
   </si>
   <si>
     <t>گزارش آماری و تفضیلی فروش یک کالا و با کلیه کالاها در بازه تاریخی قابل تنظیم</t>
   </si>
   <si>
-    <t>در گزارشات - تاریخچه ، در عناوین عملیات بهتر است این اصلاحات انجام شود :</t>
-  </si>
-  <si>
-    <t>بسته بندی نشده : ورود کالای بسته بندی نشده</t>
-  </si>
-  <si>
-    <t>بسته بندی شده : انجام بسته بندی</t>
-  </si>
-  <si>
-    <t>فروخته شده : فروش</t>
-  </si>
-  <si>
-    <t>برگشت از فروش</t>
-  </si>
-  <si>
-    <t>seperator</t>
-  </si>
-  <si>
-    <t>export to excel</t>
-  </si>
-  <si>
-    <t>conflict</t>
+    <t>edite dastie db</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>enter in password</t>
   </si>
 </sst>
 </file>
@@ -86,7 +63,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,12 +82,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -124,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -138,15 +109,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +409,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1">
         <v>23243</v>
       </c>
@@ -449,112 +419,79 @@
         <v>23242</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>0</v>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>13</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B20"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B21"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="B22"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B11">

</xml_diff>